<commit_message>
360 flip late kickflip
</commit_message>
<xml_diff>
--- a/assets/keyframes/keyframes.xlsx
+++ b/assets/keyframes/keyframes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG28"/>
+  <dimension ref="A1:AR28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -530,6 +530,39 @@
       <c r="AG1" s="1" t="n">
         <v>49.6</v>
       </c>
+      <c r="AH1" s="1" t="n">
+        <v>50.6</v>
+      </c>
+      <c r="AI1" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="AJ1" s="1" t="n">
+        <v>52.9</v>
+      </c>
+      <c r="AK1" s="1" t="n">
+        <v>53.2</v>
+      </c>
+      <c r="AL1" s="1" t="n">
+        <v>57.2</v>
+      </c>
+      <c r="AM1" s="1" t="n">
+        <v>58.2</v>
+      </c>
+      <c r="AN1" s="1" t="n">
+        <v>59.2</v>
+      </c>
+      <c r="AO1" s="1" t="n">
+        <v>61.5</v>
+      </c>
+      <c r="AP1" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="AQ1" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="AR1" s="1" t="n">
+        <v>76.59999999999999</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -625,13 +658,46 @@
         <v>0.2</v>
       </c>
       <c r="AE2" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="AF2" t="n">
         <v>0.1</v>
       </c>
       <c r="AG2" t="n">
         <v>0.2</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>-0.8</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -728,13 +794,46 @@
         <v>0.2</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="AF3" t="n">
         <v>0.2</v>
       </c>
       <c r="AG3" t="n">
         <v>0.1</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -831,13 +930,46 @@
         <v>1.1</v>
       </c>
       <c r="AE4" t="n">
-        <v>1</v>
+        <v>1.1</v>
       </c>
       <c r="AF4" t="n">
         <v>1</v>
       </c>
       <c r="AG4" t="n">
         <v>1</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>-5</v>
       </c>
     </row>
     <row r="5">
@@ -942,6 +1074,39 @@
       <c r="AG5" t="n">
         <v>0</v>
       </c>
+      <c r="AH5" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -986,7 +1151,7 @@
         <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="O6" t="n">
         <v>0.5</v>
@@ -1044,6 +1209,39 @@
       </c>
       <c r="AG6" t="n">
         <v>0.1</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -1148,6 +1346,39 @@
       <c r="AG7" t="n">
         <v>0</v>
       </c>
+      <c r="AH7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>-10</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1251,6 +1482,39 @@
       <c r="AG8" t="n">
         <v>3</v>
       </c>
+      <c r="AH8" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>3</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>3</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AR8" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1354,6 +1618,39 @@
       <c r="AG9" t="n">
         <v>0</v>
       </c>
+      <c r="AH9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>13.2</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>12.6</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>12.6</v>
+      </c>
+      <c r="AR9" t="n">
+        <v>12.6</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1457,6 +1754,39 @@
       <c r="AG10" t="n">
         <v>0</v>
       </c>
+      <c r="AH10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="AP10" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="AQ10" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="AR10" t="n">
+        <v>6.3</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -1560,6 +1890,39 @@
       <c r="AG11" t="n">
         <v>0</v>
       </c>
+      <c r="AH11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>-0.8</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>-0.4</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -1663,6 +2026,39 @@
       <c r="AG12" t="n">
         <v>0.2</v>
       </c>
+      <c r="AH12" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AI12" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ12" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR12" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -1766,6 +2162,39 @@
       <c r="AG13" t="n">
         <v>0</v>
       </c>
+      <c r="AH13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK13" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="AL13" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AM13" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AP13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -1869,6 +2298,39 @@
       <c r="AG14" t="n">
         <v>0</v>
       </c>
+      <c r="AH14" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AI14" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AJ14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN14" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO14" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AP14" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AQ14" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AR14" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -1913,7 +2375,7 @@
         <v>0</v>
       </c>
       <c r="N15" t="n">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="O15" t="n">
         <v>0</v>
@@ -1971,6 +2433,39 @@
       </c>
       <c r="AG15" t="n">
         <v>-0.3</v>
+      </c>
+      <c r="AH15" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AI15" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AJ15" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK15" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AL15" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AM15" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AN15" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AP15" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AQ15" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AR15" t="n">
+        <v>-0.1</v>
       </c>
     </row>
     <row r="16">
@@ -2075,6 +2570,39 @@
       <c r="AG16" t="n">
         <v>0.3</v>
       </c>
+      <c r="AH16" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AI16" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AJ16" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AK16" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AL16" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AM16" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AN16" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AO16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP16" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ16" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR16" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -2119,7 +2647,7 @@
         <v>-0.31</v>
       </c>
       <c r="N17" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="O17" t="n">
         <v>0.4</v>
@@ -2177,6 +2705,39 @@
       </c>
       <c r="AG17" t="n">
         <v>-0.04</v>
+      </c>
+      <c r="AH17" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="AI17" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="AJ17" t="n">
+        <v>-0.31</v>
+      </c>
+      <c r="AK17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL17" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AM17" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AN17" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AO17" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AP17" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="AQ17" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="AR17" t="n">
+        <v>-0.02</v>
       </c>
     </row>
     <row r="18">
@@ -2281,6 +2842,39 @@
       <c r="AG18" t="n">
         <v>0.1</v>
       </c>
+      <c r="AH18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ18" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="AK18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ18" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
@@ -2325,10 +2919,10 @@
         <v>0</v>
       </c>
       <c r="N19" t="n">
-        <v>0</v>
+        <v>-0.3</v>
       </c>
       <c r="O19" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="P19" t="n">
         <v>0</v>
@@ -2383,6 +2977,39 @@
       </c>
       <c r="AG19" t="n">
         <v>0.4</v>
+      </c>
+      <c r="AH19" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AI19" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AJ19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AM19" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AN19" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AO19" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="AP19" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AQ19" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AR19" t="n">
+        <v>0.7</v>
       </c>
     </row>
     <row r="20">
@@ -2428,10 +3055,10 @@
         <v>0.43</v>
       </c>
       <c r="N20" t="n">
-        <v>0</v>
+        <v>-0.1</v>
       </c>
       <c r="O20" t="n">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="P20" t="n">
         <v>0.1</v>
@@ -2486,6 +3113,39 @@
       </c>
       <c r="AG20" t="n">
         <v>-0.5</v>
+      </c>
+      <c r="AH20" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AI20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ20" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="AK20" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AL20" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AM20" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AN20" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AO20" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AP20" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AQ20" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AR20" t="n">
+        <v>0.1</v>
       </c>
     </row>
     <row r="21">
@@ -2590,6 +3250,39 @@
       <c r="AG21" t="n">
         <v>0</v>
       </c>
+      <c r="AH21" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AI21" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AJ21" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AK21" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AL21" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AM21" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AN21" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AO21" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AP21" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AQ21" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AR21" t="n">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
@@ -2634,10 +3327,10 @@
         <v>0.8</v>
       </c>
       <c r="N22" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="O22" t="n">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="P22" t="n">
         <v>0.3</v>
@@ -2692,6 +3385,39 @@
       </c>
       <c r="AG22" t="n">
         <v>0.3</v>
+      </c>
+      <c r="AH22" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AI22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ22" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AK22" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AL22" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AM22" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="AN22" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AO22" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="AP22" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AQ22" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AR22" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="23">
@@ -2737,7 +3463,7 @@
         <v>1</v>
       </c>
       <c r="N23" t="n">
-        <v>-1.5</v>
+        <v>-1</v>
       </c>
       <c r="O23" t="n">
         <v>-0.5</v>
@@ -2795,6 +3521,39 @@
       </c>
       <c r="AG23" t="n">
         <v>-0.6</v>
+      </c>
+      <c r="AH23" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AI23" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AJ23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK23" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AL23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO23" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AP23" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AQ23" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AR23" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="24">
@@ -2899,6 +3658,39 @@
       <c r="AG24" t="n">
         <v>-0.3</v>
       </c>
+      <c r="AH24" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="AI24" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="AJ24" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AK24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP24" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="AQ24" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="AR24" t="n">
+        <v>-0.5</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
@@ -3002,6 +3794,39 @@
       <c r="AG25" t="n">
         <v>0.1</v>
       </c>
+      <c r="AH25" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AI25" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AJ25" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AK25" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AL25" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AM25" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AN25" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AO25" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="AP25" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AQ25" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AR25" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
@@ -3105,6 +3930,39 @@
       <c r="AG26" t="n">
         <v>0</v>
       </c>
+      <c r="AH26" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AI26" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AJ26" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AK26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL26" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="AM26" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AN26" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AO26" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AP26" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AQ26" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AR26" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
@@ -3208,6 +4066,39 @@
       <c r="AG27" t="n">
         <v>0.2</v>
       </c>
+      <c r="AH27" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AI27" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AJ27" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="AK27" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="AL27" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AM27" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AN27" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AO27" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="AP27" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AQ27" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AR27" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
@@ -3252,7 +4143,7 @@
         <v>1.1</v>
       </c>
       <c r="N28" t="n">
-        <v>-0.8</v>
+        <v>0</v>
       </c>
       <c r="O28" t="n">
         <v>-0.3</v>
@@ -3310,6 +4201,39 @@
       </c>
       <c r="AG28" t="n">
         <v>0.3</v>
+      </c>
+      <c r="AH28" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AI28" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AJ28" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="AK28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM28" t="n">
+        <v>-0.3</v>
+      </c>
+      <c r="AN28" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="AO28" t="n">
+        <v>-0.8</v>
+      </c>
+      <c r="AP28" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AQ28" t="n">
+        <v>-0.1</v>
+      </c>
+      <c r="AR28" t="n">
+        <v>-0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>